<commit_message>
Updated Exposé and Timeline
</commit_message>
<xml_diff>
--- a/00_general_info/Master_Timeline.xlsx
+++ b/00_general_info/Master_Timeline.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\Masterarbeit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\Master CAU\00_general_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Aktivität</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Version</t>
   </si>
   <si>
-    <t xml:space="preserve">Fragestellung </t>
-  </si>
-  <si>
     <t xml:space="preserve">Auswertung </t>
   </si>
   <si>
@@ -53,16 +50,22 @@
     <t>erstes Literaturstudium</t>
   </si>
   <si>
-    <t>Skript zum Einlesen der Daten</t>
-  </si>
-  <si>
     <t>Skript für die Verarbeitung der Daten</t>
   </si>
   <si>
-    <t>Betrachtung der Daten und Exposé</t>
-  </si>
-  <si>
     <t>Skript für FOOOF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Betrachtung der Daten </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fragestellung überlegen </t>
+  </si>
+  <si>
+    <t>Skript zum Einlesen der Daten + Vorbereitung/ weitere Recherche</t>
+  </si>
+  <si>
+    <t>Abgabe</t>
   </si>
 </sst>
 </file>
@@ -390,154 +393,168 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.109375" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="1" max="1" width="54.5546875" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="F2" s="2">
-        <v>44224</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E2" s="2">
+        <v>44342</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2">
+        <v>44263</v>
+      </c>
+      <c r="C4">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2">
+        <v>44285</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2">
+        <v>44277</v>
+      </c>
+      <c r="C5">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2">
+        <v>44285</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2">
+        <v>44286</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2">
+        <v>44299</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2">
+        <v>44299</v>
+      </c>
+      <c r="C7">
+        <v>48</v>
+      </c>
+      <c r="D7" s="2">
+        <v>44347</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2">
-        <v>44263</v>
-      </c>
-      <c r="D4">
-        <v>23</v>
-      </c>
-      <c r="E4" s="2">
-        <v>44285</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+      <c r="B8" s="2">
+        <v>44347</v>
+      </c>
+      <c r="C8">
+        <v>31</v>
+      </c>
+      <c r="D8" s="2">
+        <v>44378</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>44378</v>
+      </c>
+      <c r="C9">
+        <v>62</v>
+      </c>
+      <c r="D9" s="2">
+        <v>44440</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2">
-        <v>44277</v>
-      </c>
-      <c r="D5">
-        <v>9</v>
-      </c>
-      <c r="E5" s="2">
-        <v>44285</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2">
-        <v>44286</v>
-      </c>
-      <c r="D6">
-        <v>12</v>
-      </c>
-      <c r="E6" s="2">
-        <v>44299</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="2">
-        <v>44299</v>
-      </c>
-      <c r="D7">
-        <v>48</v>
-      </c>
-      <c r="E7" s="2">
-        <v>44347</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="2">
-        <v>44347</v>
-      </c>
-      <c r="D8">
-        <v>31</v>
-      </c>
-      <c r="E8" s="2">
-        <v>44378</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="2">
-        <v>44378</v>
-      </c>
-      <c r="D9">
-        <v>62</v>
-      </c>
-      <c r="E9" s="2">
+      <c r="B10" s="2">
         <v>44440</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+      <c r="C10">
+        <v>122</v>
+      </c>
+      <c r="D10" s="2">
+        <v>44562</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="2">
-        <v>44440</v>
-      </c>
-      <c r="D10">
-        <v>122</v>
-      </c>
-      <c r="E10" s="2">
+      <c r="B11" s="2">
         <v>44562</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="2">
-        <v>44562</v>
-      </c>
-      <c r="D11">
-        <v>89</v>
-      </c>
-      <c r="E11" s="2">
+      <c r="C11">
+        <v>84</v>
+      </c>
+      <c r="D11" s="2">
+        <v>44645</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2">
+        <v>44646</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2">
         <v>44650</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>